<commit_message>
Finished testing and updated manual
</commit_message>
<xml_diff>
--- a/Testing Matrix.xlsx
+++ b/Testing Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/DropBox/dropbox/EWHO/Application Development/MasterDarkMaker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/DropBox/dropbox/EWHO/Application Development/MasterBiasMaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971BEF33-DD8E-4646-BC67-AA073F0ADFC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C5DB42-BB31-CA45-8E1E-E9F38667EF82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21660" yWindow="540" windowWidth="11580" windowHeight="10580" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
+    <workbookView xWindow="34760" yWindow="1440" windowWidth="15900" windowHeight="10540" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,32 +33,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
   <si>
     <t>Single-file testing</t>
   </si>
   <si>
-    <t>No Precal</t>
-  </si>
-  <si>
-    <t>Pedestal</t>
-  </si>
-  <si>
-    <t>Auto</t>
-  </si>
-  <si>
-    <t>Fixed file</t>
-  </si>
-  <si>
     <t>Mean</t>
   </si>
   <si>
     <t>Median</t>
   </si>
   <si>
-    <t>Sigma</t>
-  </si>
-  <si>
     <t>Groups Testing</t>
   </si>
   <si>
@@ -68,13 +53,40 @@
     <t>✘</t>
   </si>
   <si>
-    <t>Two tests: complet and cancel</t>
-  </si>
-  <si>
     <t>MinMax 1</t>
   </si>
   <si>
     <t>MinMax 2</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>1x1</t>
+  </si>
+  <si>
+    <t>2x2</t>
+  </si>
+  <si>
+    <t>3x3</t>
+  </si>
+  <si>
+    <t>Invalid mix</t>
+  </si>
+  <si>
+    <t>Sigma 2</t>
+  </si>
+  <si>
+    <t>Sigma 3</t>
+  </si>
+  <si>
+    <t>Dispose</t>
   </si>
 </sst>
 </file>
@@ -449,229 +461,247 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47930263-E802-DC48-8BED-3FA036517820}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="6" width="10.83203125" style="1"/>
-    <col min="7" max="7" width="4.1640625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="4.1640625" customWidth="1"/>
+    <col min="2" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="4.1640625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="K2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="J2" s="3" t="s">
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change temperature tolerance to "bandwidth" for MeanShift clustering (haven't implemented the clustering yet)
</commit_message>
<xml_diff>
--- a/Testing Matrix.xlsx
+++ b/Testing Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/DropBox/dropbox/EWHO/Application Development/MasterBiasMaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C5DB42-BB31-CA45-8E1E-E9F38667EF82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912CA28A-593A-344E-8A47-52D94608EF3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34760" yWindow="1440" windowWidth="15900" windowHeight="10540" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
+    <workbookView xWindow="380" yWindow="1080" windowWidth="16540" windowHeight="17320" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="20">
   <si>
     <t>Single-file testing</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Dispose</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Command Line</t>
   </si>
 </sst>
 </file>
@@ -461,247 +467,383 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47930263-E802-DC48-8BED-3FA036517820}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A2:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="7" width="10.83203125" style="1"/>
-    <col min="8" max="8" width="4.1640625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="4.1640625" customWidth="1"/>
+    <col min="3" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="4.1640625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="K2" s="3" t="s">
+      <c r="L3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="L4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="B3" s="1" t="s">
+    <row r="5" spans="1:12">
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
+    <row r="6" spans="1:12">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" t="s">
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="B11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="B11" s="1" t="s">
+    <row r="13" spans="1:12">
+      <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
-      <c r="A12" t="s">
+    <row r="14" spans="1:12">
+      <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" t="s">
+      <c r="C14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" t="s">
+      <c r="C15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="B16" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" t="s">
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="C30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improve information displayed on console and in file names
</commit_message>
<xml_diff>
--- a/Testing Matrix.xlsx
+++ b/Testing Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/DropBox/dropbox/EWHO/Application Development/MasterBiasMaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912CA28A-593A-344E-8A47-52D94608EF3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0DBFF0-0352-3249-B57E-371349C461CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="1080" windowWidth="16540" windowHeight="17320" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
+    <workbookView xWindow="53340" yWindow="2980" windowWidth="16540" windowHeight="17320" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="22">
   <si>
     <t>Single-file testing</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Command Line</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Ignore</t>
   </si>
 </sst>
 </file>
@@ -467,38 +473,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47930263-E802-DC48-8BED-3FA036517820}">
-  <dimension ref="A2:L34"/>
+  <dimension ref="A2:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="8" width="10.83203125" style="1"/>
-    <col min="9" max="9" width="4.1640625" style="1" customWidth="1"/>
-    <col min="10" max="11" width="4.1640625" customWidth="1"/>
+    <col min="3" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="4.1640625" style="1" customWidth="1"/>
+    <col min="11" max="12" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="L4" s="3" t="s">
+      <c r="M3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="M4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
@@ -517,8 +523,11 @@
       <c r="H5" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -540,9 +549,12 @@
       <c r="H6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="I6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -564,9 +576,12 @@
       <c r="H7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="I7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -588,9 +603,12 @@
       <c r="H8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="I8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -603,13 +621,14 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="11" spans="1:13">
       <c r="B11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
@@ -628,8 +647,11 @@
       <c r="H13" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="I13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -651,9 +673,12 @@
       <c r="H14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="I14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:13">
       <c r="B15" t="s">
         <v>9</v>
       </c>
@@ -672,10 +697,15 @@
       <c r="G15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="H15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -685,165 +715,305 @@
       <c r="D16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="E16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="B20" t="s">
+    <row r="21" spans="1:10">
+      <c r="B21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="C22" s="1" t="s">
+    <row r="23" spans="1:10">
+      <c r="C23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="B23" t="s">
+    <row r="24" spans="1:10">
+      <c r="B24" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="B24" t="s">
+      <c r="C24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="B25" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="B25" t="s">
+      <c r="C25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="B26" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="B26" t="s">
+      <c r="C26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="B27" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="B28" t="s">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="B29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
-      <c r="C30" s="1" t="s">
+    <row r="31" spans="1:10">
+      <c r="C31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="B31" t="s">
+    <row r="32" spans="1:10">
+      <c r="B32" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="B32" t="s">
+      <c r="C32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="2:8">
-      <c r="B33" t="s">
+      <c r="C33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="2:8">
-      <c r="B34" t="s">
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>